<commit_message>
Preparing for remembering last input in local storag.
</commit_message>
<xml_diff>
--- a/underlag.xlsx
+++ b/underlag.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ArtComputer.se" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.000\ &quot;kr&quot;_-;\-* #,##0.000\ &quot;kr&quot;_-;_-* &quot;-&quot;???\ &quot;kr&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000\ &quot;kr&quot;_-;\-* #,##0.000\ &quot;kr&quot;_-;_-* &quot;-&quot;???\ &quot;kr&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -227,10 +227,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -245,13 +259,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,8 +282,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -278,11 +290,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="19">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -561,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,6 +805,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -784,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="L5" sqref="L5:L22"/>
     </sheetView>
   </sheetViews>
@@ -823,20 +852,20 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F3" s="11"/>
       <c r="K3" s="18"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:16" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -872,16 +901,16 @@
       <c r="K4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="19" t="s">
         <v>28</v>
       </c>
     </row>
@@ -924,19 +953,19 @@
         <f>C5*0.01/12</f>
         <v>8180.833333333333</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="22">
         <f>K5*D5</f>
         <v>704.94240833333333</v>
       </c>
-      <c r="M5" s="22" t="str">
+      <c r="M5" s="20" t="str">
         <f>IF(G5&lt;=0.25,"OK",IF(G5&lt;=0.5,"Gränsfall","Se upp!"))</f>
         <v>OK</v>
       </c>
-      <c r="N5" s="23" t="str">
+      <c r="N5" s="21" t="str">
         <f>IF(I5&gt;=9000,"Hög",IF(I5&gt;=6000,"Måttlig till hög",IF(I5&gt;3000,"Måttlig till låg","Låg")))</f>
         <v>Hög</v>
       </c>
-      <c r="O5" s="23" t="str">
+      <c r="O5" s="21" t="str">
         <f>IF(J5&gt;=900,"Hög",IF(J5&gt;=650,"Måttlig till hög",IF(J5&gt;300,"Måttlig till låg","Låg")))</f>
         <v>Måttlig till hög</v>
       </c>
@@ -972,19 +1001,19 @@
         <f t="shared" ref="K6:K22" si="4">C6*0.01/12</f>
         <v>0</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="22">
         <f t="shared" ref="L6:L22" si="5">K6*D6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="22" t="str">
+      <c r="M6" s="20" t="str">
         <f t="shared" ref="M6:M22" si="6">IF(G6&lt;=0.25,"OK",IF(G6&lt;=0.5,"Gränsfall","Se upp!"))</f>
         <v>Se upp!</v>
       </c>
-      <c r="N6" s="23" t="str">
+      <c r="N6" s="21" t="str">
         <f t="shared" ref="N6:N22" si="7">IF(I6&gt;=9000,"Hög",IF(I6&gt;=6000,"Måttlig till hög",IF(I6&gt;3000,"Måttlig till låg","Låg")))</f>
         <v>Hög</v>
       </c>
-      <c r="O6" s="23" t="str">
+      <c r="O6" s="21" t="str">
         <f t="shared" ref="O6:O22" si="8">IF(J6&gt;=900,"Hög",IF(J6&gt;=650,"Måttlig till hög",IF(J6&gt;300,"Måttlig till låg","Låg")))</f>
         <v>Hög</v>
       </c>
@@ -1020,19 +1049,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M7" s="22" t="str">
+      <c r="M7" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N7" s="23" t="str">
+      <c r="N7" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O7" s="23" t="str">
+      <c r="O7" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1068,19 +1097,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M8" s="22" t="str">
+      <c r="M8" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N8" s="23" t="str">
+      <c r="N8" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O8" s="23" t="str">
+      <c r="O8" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1116,19 +1145,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L9" s="24">
+      <c r="L9" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M9" s="22" t="str">
+      <c r="M9" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N9" s="23" t="str">
+      <c r="N9" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O9" s="23" t="str">
+      <c r="O9" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1164,19 +1193,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L10" s="24">
+      <c r="L10" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M10" s="22" t="str">
+      <c r="M10" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N10" s="23" t="str">
+      <c r="N10" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O10" s="23" t="str">
+      <c r="O10" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1212,19 +1241,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L11" s="24">
+      <c r="L11" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M11" s="22" t="str">
+      <c r="M11" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N11" s="23" t="str">
+      <c r="N11" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O11" s="23" t="str">
+      <c r="O11" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1260,19 +1289,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M12" s="22" t="str">
+      <c r="M12" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N12" s="23" t="str">
+      <c r="N12" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O12" s="23" t="str">
+      <c r="O12" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1308,19 +1337,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M13" s="22" t="str">
+      <c r="M13" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N13" s="23" t="str">
+      <c r="N13" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O13" s="23" t="str">
+      <c r="O13" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1356,19 +1385,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L14" s="24">
+      <c r="L14" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M14" s="22" t="str">
+      <c r="M14" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N14" s="23" t="str">
+      <c r="N14" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O14" s="23" t="str">
+      <c r="O14" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1404,19 +1433,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M15" s="22" t="str">
+      <c r="M15" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N15" s="23" t="str">
+      <c r="N15" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O15" s="23" t="str">
+      <c r="O15" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1452,19 +1481,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L16" s="24">
+      <c r="L16" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M16" s="22" t="str">
+      <c r="M16" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N16" s="23" t="str">
+      <c r="N16" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O16" s="23" t="str">
+      <c r="O16" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1500,19 +1529,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L17" s="24">
+      <c r="L17" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M17" s="22" t="str">
+      <c r="M17" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N17" s="23" t="str">
+      <c r="N17" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O17" s="23" t="str">
+      <c r="O17" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1548,19 +1577,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L18" s="24">
+      <c r="L18" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M18" s="22" t="str">
+      <c r="M18" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N18" s="23" t="str">
+      <c r="N18" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O18" s="23" t="str">
+      <c r="O18" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1596,19 +1625,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L19" s="24">
+      <c r="L19" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M19" s="22" t="str">
+      <c r="M19" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N19" s="23" t="str">
+      <c r="N19" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O19" s="23" t="str">
+      <c r="O19" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1644,19 +1673,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L20" s="24">
+      <c r="L20" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M20" s="22" t="str">
+      <c r="M20" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N20" s="23" t="str">
+      <c r="N20" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O20" s="23" t="str">
+      <c r="O20" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1692,19 +1721,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M21" s="22" t="str">
+      <c r="M21" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N21" s="23" t="str">
+      <c r="N21" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O21" s="23" t="str">
+      <c r="O21" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>
@@ -1740,19 +1769,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L22" s="24">
+      <c r="L22" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M22" s="22" t="str">
+      <c r="M22" s="20" t="str">
         <f t="shared" si="6"/>
         <v>Se upp!</v>
       </c>
-      <c r="N22" s="23" t="str">
+      <c r="N22" s="21" t="str">
         <f t="shared" si="7"/>
         <v>Hög</v>
       </c>
-      <c r="O22" s="23" t="str">
+      <c r="O22" s="21" t="str">
         <f t="shared" si="8"/>
         <v>Hög</v>
       </c>

</xml_diff>